<commit_message>
Small Product Backlog change.
</commit_message>
<xml_diff>
--- a/deliverable5/Product_Backlog_RootDigital.xlsx
+++ b/deliverable5/Product_Backlog_RootDigital.xlsx
@@ -307,11 +307,11 @@
   </sheetPr>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="59"/>
@@ -732,7 +732,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F21" s="7" t="n">
         <v>8</v>

</xml_diff>